<commit_message>
PArse to precision 3
</commit_message>
<xml_diff>
--- a/public/Door Schedule w_ Images.xlsx
+++ b/public/Door Schedule w_ Images.xlsx
@@ -391,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -405,6 +405,13 @@
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
+    </border>
+    <border diagonalUp="true" diagonalDown="true">
+      <left style="mediumDashed"/>
+      <right style="mediumDashed"/>
+      <top/>
+      <bottom/>
+      <diagonal style="mediumDashed"/>
     </border>
   </borders>
   <cellStyleXfs count="20">
@@ -432,104 +439,112 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -616,9 +631,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -632,7 +647,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="1809720"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -653,9 +668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -669,7 +684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="2457720"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -690,9 +705,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -706,7 +721,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="3105360"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -727,9 +742,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -743,7 +758,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="3753000"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -764,9 +779,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -780,7 +795,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="4400640"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -801,9 +816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -817,7 +832,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="5048280"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -838,9 +853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -854,7 +869,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="5695920"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -875,9 +890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -891,7 +906,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="6343920"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -912,9 +927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -928,7 +943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="6991560"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -949,9 +964,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -965,7 +980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="7639200"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -986,9 +1001,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,7 +1017,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="8286840"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1023,9 +1038,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>856800</xdr:colOff>
+      <xdr:colOff>856440</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1039,7 +1054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="8934480"/>
-          <a:ext cx="380520" cy="742680"/>
+          <a:ext cx="380160" cy="742320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1168,909 +1183,909 @@
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E16"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="35.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="26.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="76.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="35.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="76.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="2" t="s">
+      <c r="T2" s="5"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="3"/>
+      <c r="X2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="13"/>
-      <c r="X3" s="12" t="s">
+      <c r="W3" s="14"/>
+      <c r="X3" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="n">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="16" t="n">
+      <c r="E4" s="17" t="n">
         <v>60.5</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="18" t="n">
         <v>98.4166666666667</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="18" t="n">
         <v>1.71875</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15" t="n">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="J4" s="18" t="n">
+      <c r="J4" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="15" t="n">
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="N4" s="15" t="n">
+      <c r="N4" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="O4" s="15" t="n">
+      <c r="O4" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="P4" s="15" t="n">
+      <c r="P4" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="Q4" s="18" t="n">
+      <c r="Q4" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="R4" s="18" t="n">
+      <c r="R4" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="S4" s="18"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15" t="n">
+      <c r="S4" s="19"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21" t="n">
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="22" t="n">
+      <c r="F5" s="24" t="n">
         <v>6.66666666666667</v>
       </c>
-      <c r="G5" s="22" t="n">
+      <c r="G5" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="Q5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="23" t="s">
+      <c r="R5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="24"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="19" t="s">
+      <c r="S5" s="26"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="V5" s="23" t="s">
+      <c r="V5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="W5" s="23" t="s">
+      <c r="W5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="X5" s="24"/>
+      <c r="X5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="16" t="n">
+      <c r="D6" s="22"/>
+      <c r="E6" s="17" t="n">
         <v>2.83333333333333</v>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="G6" s="22" t="n">
+      <c r="G6" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="P6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="S6" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="T6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="U6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="V6" s="23" t="s">
+      <c r="V6" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="W6" s="23" t="s">
+      <c r="W6" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="23" t="s">
+      <c r="X6" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="16" t="n">
+      <c r="D7" s="22"/>
+      <c r="E7" s="17" t="n">
         <v>2.83333333333333</v>
       </c>
-      <c r="F7" s="22" t="n">
+      <c r="F7" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="G7" s="22" t="n">
+      <c r="G7" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q7" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="S7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="U7" s="19" t="s">
+      <c r="U7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="V7" s="23" t="s">
+      <c r="V7" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="W7" s="23" t="s">
+      <c r="W7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="X7" s="23" t="s">
+      <c r="X7" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="16" t="n">
+      <c r="D8" s="22"/>
+      <c r="E8" s="17" t="n">
         <v>2.83333333333333</v>
       </c>
-      <c r="F8" s="22" t="n">
+      <c r="F8" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="G8" s="22" t="n">
+      <c r="G8" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="Q8" s="23" t="s">
+      <c r="Q8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="23" t="s">
+      <c r="S8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="T8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="19" t="s">
+      <c r="U8" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="V8" s="23" t="s">
+      <c r="V8" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="W8" s="23" t="s">
+      <c r="W8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="X8" s="23" t="s">
+      <c r="X8" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21" t="n">
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="F9" s="22" t="n">
+      <c r="F9" s="24" t="n">
         <v>11.75</v>
       </c>
-      <c r="G9" s="22" t="n">
+      <c r="G9" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="23" t="s">
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="23" t="s">
+      <c r="R9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="S9" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="T9" s="19" t="s">
+      <c r="T9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="U9" s="19" t="s">
+      <c r="U9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="23" t="s">
+      <c r="V9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="W9" s="23" t="s">
+      <c r="W9" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="X9" s="23" t="s">
+      <c r="X9" s="25" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="n">
+      <c r="D10" s="22"/>
+      <c r="E10" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="F10" s="22" t="n">
+      <c r="F10" s="24" t="n">
         <v>11.75</v>
       </c>
-      <c r="G10" s="22" t="n">
+      <c r="G10" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="23" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="S10" s="23" t="s">
+      <c r="S10" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="T10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="U10" s="19" t="s">
+      <c r="U10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="V10" s="23" t="s">
+      <c r="V10" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="W10" s="23" t="s">
+      <c r="W10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="X10" s="23" t="s">
+      <c r="X10" s="25" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="16" t="n">
+      <c r="D11" s="22"/>
+      <c r="E11" s="17" t="n">
         <v>3.66666666666667</v>
       </c>
-      <c r="F11" s="22" t="n">
+      <c r="F11" s="24" t="n">
         <v>8.83333333333333</v>
       </c>
-      <c r="G11" s="22" t="n">
+      <c r="G11" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23" t="s">
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="19" t="s">
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="V11" s="24"/>
-      <c r="W11" s="23" t="s">
+      <c r="V11" s="26"/>
+      <c r="W11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="X11" s="23" t="s">
+      <c r="X11" s="25" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21" t="n">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="22" t="n">
+      <c r="F12" s="24" t="n">
         <v>6.66666666666667</v>
       </c>
-      <c r="G12" s="22" t="n">
+      <c r="G12" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23" t="s">
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="19" t="s">
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="V12" s="24"/>
-      <c r="W12" s="23" t="s">
+      <c r="V12" s="26"/>
+      <c r="W12" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="X12" s="23" t="s">
+      <c r="X12" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21" t="n">
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="22" t="n">
+      <c r="F13" s="24" t="n">
         <v>6.66666666666667</v>
       </c>
-      <c r="G13" s="22" t="n">
+      <c r="G13" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23" t="s">
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="19" t="s">
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="V13" s="24"/>
-      <c r="W13" s="23" t="s">
+      <c r="V13" s="26"/>
+      <c r="W13" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="X13" s="23" t="s">
+      <c r="X13" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21" t="n">
+      <c r="D14" s="22"/>
+      <c r="E14" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="22" t="n">
+      <c r="F14" s="24" t="n">
         <v>6.66666666666667</v>
       </c>
-      <c r="G14" s="22" t="n">
+      <c r="G14" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23" t="s">
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="19" t="s">
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="V14" s="24"/>
-      <c r="W14" s="23" t="s">
+      <c r="V14" s="26"/>
+      <c r="W14" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="X14" s="23" t="s">
+      <c r="X14" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="16" t="n">
+      <c r="D15" s="22"/>
+      <c r="E15" s="17" t="n">
         <v>3.33333333333333</v>
       </c>
-      <c r="F15" s="22" t="n">
+      <c r="F15" s="24" t="n">
         <v>6.66666666666667</v>
       </c>
-      <c r="G15" s="22" t="n">
+      <c r="G15" s="24" t="n">
         <v>0.114583333333333</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23" t="s">
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="19" t="s">
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="V15" s="24"/>
-      <c r="W15" s="23" t="s">
+      <c r="V15" s="26"/>
+      <c r="W15" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="X15" s="23" t="s">
+      <c r="X15" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21" t="n">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="22" t="n">
+      <c r="F16" s="24" t="n">
         <v>8.75</v>
       </c>
-      <c r="G16" s="22" t="n">
+      <c r="G16" s="24" t="n">
         <v>0.145833333333333</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23" t="s">
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="19" t="s">
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="23" t="s">
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="25" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2084,6 +2099,9 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="Width"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2091,6 +2109,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>